<commit_message>
updated more analysis dates
</commit_message>
<xml_diff>
--- a/data/uwf_yr3_analysis_dates.xlsx
+++ b/data/uwf_yr3_analysis_dates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\wqx-data-upload-tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD1D078-09F8-4660-97E8-7C2B1B931898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3F4410-5614-4180-BA69-409A4CBB4533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{11D46821-4D73-4E39-90CE-C70DBFE516E7}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$165</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="29">
   <si>
     <t>Analyte</t>
   </si>
@@ -132,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,25 +145,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -175,19 +163,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B6ABD3C4-2763-435D-9037-444FE9298413}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{95198F50-8C42-4622-B773-6BFE399EC950}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -519,11 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A68A17-021F-4C89-9F43-C50D4EDC1708}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140:B141"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="K104" sqref="K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +520,8 @@
     <col min="3" max="3" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" customWidth="1"/>
+    <col min="19" max="24" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,7 +541,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -563,7 +552,7 @@
         <v>45595</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -574,7 +563,7 @@
         <v>45595</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -585,7 +574,7 @@
         <v>45742</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -596,7 +585,7 @@
         <v>45742</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -607,7 +596,7 @@
         <v>45742</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -618,7 +607,7 @@
         <v>45742</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -629,7 +618,7 @@
         <v>45749</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -640,7 +629,7 @@
         <v>45749</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -651,7 +640,7 @@
         <v>45749</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -662,7 +651,7 @@
         <v>45749</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -673,7 +662,7 @@
         <v>45756</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -684,7 +673,7 @@
         <v>45756</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -695,7 +684,7 @@
         <v>45756</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -706,7 +695,7 @@
         <v>45756</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -717,7 +706,7 @@
         <v>45771</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -728,7 +717,7 @@
         <v>45771</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -739,7 +728,7 @@
         <v>45771</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -750,7 +739,7 @@
         <v>45771</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -761,7 +750,7 @@
         <v>45770</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -772,7 +761,7 @@
         <v>45770</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -783,7 +772,7 @@
         <v>45770</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -794,7 +783,7 @@
         <v>45770</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -805,7 +794,7 @@
         <v>45806</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -816,7 +805,7 @@
         <v>45806</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -827,7 +816,7 @@
         <v>45806</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -838,7 +827,7 @@
         <v>45806</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -893,7 +882,7 @@
         <v>45897</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -904,7 +893,7 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -926,7 +915,7 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -943,7 +932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -960,7 +949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -977,7 +966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -994,7 +983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1011,7 +1000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1028,7 +1017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1045,7 +1034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1062,7 +1051,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1079,7 +1068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1096,7 +1085,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -1113,7 +1102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1130,7 +1119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -1147,7 +1136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1164,7 +1153,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1181,7 +1170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -1198,7 +1187,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -1215,7 +1204,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -1232,7 +1221,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -1249,7 +1238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -1266,7 +1255,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>9</v>
       </c>
@@ -1283,7 +1272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -1300,7 +1289,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -1317,7 +1306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -1334,7 +1323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -1351,7 +1340,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -1368,7 +1357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>9</v>
       </c>
@@ -1385,7 +1374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -1402,7 +1391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -1419,7 +1408,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>9</v>
       </c>
@@ -1436,7 +1425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>9</v>
       </c>
@@ -1453,7 +1442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -1470,7 +1459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>9</v>
       </c>
@@ -1487,7 +1476,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>9</v>
       </c>
@@ -1504,7 +1493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>9</v>
       </c>
@@ -1521,7 +1510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>9</v>
       </c>
@@ -1538,7 +1527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -1555,7 +1544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>9</v>
       </c>
@@ -1572,7 +1561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>9</v>
       </c>
@@ -1589,7 +1578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -1606,7 +1595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -1861,7 +1850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>24</v>
       </c>
@@ -1872,7 +1861,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>24</v>
       </c>
@@ -1894,165 +1883,197 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B94" s="3">
-        <v>45582</v>
-      </c>
-      <c r="C94" s="3"/>
-    </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>26</v>
+      </c>
+      <c r="B94" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C94" s="1">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>26</v>
       </c>
       <c r="B95" s="1">
-        <v>45582</v>
+        <v>45580</v>
       </c>
       <c r="C95" s="1">
-        <v>45582</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B96" s="3">
-        <v>45582</v>
-      </c>
-      <c r="C96" s="3"/>
-    </row>
-    <row r="97" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B97" s="3">
         <v>45580</v>
       </c>
-      <c r="C97" s="3"/>
-    </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>28</v>
+      </c>
+      <c r="B96" s="1">
+        <v>45670</v>
+      </c>
+      <c r="C96" s="1">
+        <v>45670</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97" s="1">
+        <v>45671</v>
+      </c>
+      <c r="C97" s="1">
+        <v>45671</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>26</v>
       </c>
       <c r="B98" s="1">
-        <v>45580</v>
+        <v>45768</v>
       </c>
       <c r="C98" s="1">
-        <v>45580</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B99" s="3">
-        <v>45580</v>
-      </c>
-      <c r="C99" s="3"/>
-    </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>26</v>
+      </c>
+      <c r="B99" s="1">
+        <v>45769</v>
+      </c>
+      <c r="C99" s="1">
+        <v>45769</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B100" s="1">
-        <v>45670</v>
+        <v>45861</v>
       </c>
       <c r="C100" s="1">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>45861</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>26</v>
       </c>
       <c r="B101" s="1">
-        <v>45671</v>
+        <v>45862</v>
       </c>
       <c r="C101" s="1">
-        <v>45671</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>45862</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B102" s="1">
-        <v>45768</v>
+        <v>45670</v>
       </c>
       <c r="C102" s="1">
-        <v>45768</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>45687</v>
+      </c>
+      <c r="D102" t="s">
+        <v>10</v>
+      </c>
+      <c r="E102" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B103" s="1">
-        <v>45769</v>
+        <v>45670</v>
       </c>
       <c r="C103" s="1">
-        <v>45769</v>
+        <v>45687</v>
+      </c>
+      <c r="D103" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B104" s="1">
-        <v>45861</v>
+        <v>45671</v>
       </c>
       <c r="C104" s="1">
-        <v>45861</v>
+        <v>45689</v>
+      </c>
+      <c r="D104" t="s">
+        <v>13</v>
+      </c>
+      <c r="E104" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B105" s="1">
-        <v>45862</v>
+        <v>45671</v>
       </c>
       <c r="C105" s="1">
-        <v>45862</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>45689</v>
+      </c>
+      <c r="D105" t="s">
+        <v>13</v>
+      </c>
+      <c r="E105" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>25</v>
       </c>
       <c r="B106" s="1">
-        <v>45670</v>
+        <v>45671</v>
       </c>
       <c r="C106" s="1">
         <v>45687</v>
       </c>
       <c r="D106" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E106" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>27</v>
       </c>
       <c r="B107" s="1">
-        <v>45670</v>
+        <v>45671</v>
       </c>
       <c r="C107" s="1">
         <v>45687</v>
       </c>
       <c r="D107" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>25</v>
       </c>
@@ -2060,16 +2081,16 @@
         <v>45671</v>
       </c>
       <c r="C108" s="1">
-        <v>45689</v>
+        <v>45687</v>
       </c>
       <c r="D108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E108" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>27</v>
       </c>
@@ -2077,16 +2098,16 @@
         <v>45671</v>
       </c>
       <c r="C109" s="1">
-        <v>45689</v>
+        <v>45687</v>
       </c>
       <c r="D109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E109" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>25</v>
       </c>
@@ -2097,13 +2118,13 @@
         <v>45687</v>
       </c>
       <c r="D110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E110" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>27</v>
       </c>
@@ -2114,13 +2135,13 @@
         <v>45687</v>
       </c>
       <c r="D111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E111" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>25</v>
       </c>
@@ -2128,16 +2149,16 @@
         <v>45671</v>
       </c>
       <c r="C112" s="1">
-        <v>45687</v>
+        <v>45689</v>
       </c>
       <c r="D112" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E112" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>27</v>
       </c>
@@ -2148,13 +2169,13 @@
         <v>45687</v>
       </c>
       <c r="D113" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E113" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>25</v>
       </c>
@@ -2162,16 +2183,16 @@
         <v>45671</v>
       </c>
       <c r="C114" s="1">
-        <v>45687</v>
+        <v>45689</v>
       </c>
       <c r="D114" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E114" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>27</v>
       </c>
@@ -2182,13 +2203,13 @@
         <v>45687</v>
       </c>
       <c r="D115" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E115" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>25</v>
       </c>
@@ -2199,13 +2220,13 @@
         <v>45689</v>
       </c>
       <c r="D116" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E116" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>27</v>
       </c>
@@ -2216,13 +2237,13 @@
         <v>45687</v>
       </c>
       <c r="D117" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E117" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>25</v>
       </c>
@@ -2233,13 +2254,13 @@
         <v>45689</v>
       </c>
       <c r="D118" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E118" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>27</v>
       </c>
@@ -2250,13 +2271,13 @@
         <v>45687</v>
       </c>
       <c r="D119" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E119" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>25</v>
       </c>
@@ -2267,13 +2288,13 @@
         <v>45689</v>
       </c>
       <c r="D120" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E120" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>27</v>
       </c>
@@ -2284,13 +2305,13 @@
         <v>45687</v>
       </c>
       <c r="D121" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E121" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>25</v>
       </c>
@@ -2301,13 +2322,13 @@
         <v>45689</v>
       </c>
       <c r="D122" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E122" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>27</v>
       </c>
@@ -2318,13 +2339,13 @@
         <v>45687</v>
       </c>
       <c r="D123" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E123" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>25</v>
       </c>
@@ -2335,13 +2356,13 @@
         <v>45689</v>
       </c>
       <c r="D124" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E124" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>27</v>
       </c>
@@ -2349,16 +2370,16 @@
         <v>45671</v>
       </c>
       <c r="C125" s="1">
-        <v>45687</v>
+        <v>45689</v>
       </c>
       <c r="D125" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E125" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>25</v>
       </c>
@@ -2369,13 +2390,13 @@
         <v>45689</v>
       </c>
       <c r="D126" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E126" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>27</v>
       </c>
@@ -2383,201 +2404,603 @@
         <v>45671</v>
       </c>
       <c r="C127" s="1">
-        <v>45687</v>
+        <v>45689</v>
       </c>
       <c r="D127" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E127" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B128" s="1">
-        <v>45671</v>
+        <v>45768</v>
       </c>
       <c r="C128" s="1">
-        <v>45689</v>
-      </c>
-      <c r="D128" t="s">
-        <v>17</v>
-      </c>
-      <c r="E128" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B129" s="1">
-        <v>45671</v>
+        <v>45768</v>
       </c>
       <c r="C129" s="1">
-        <v>45689</v>
-      </c>
-      <c r="D129" t="s">
-        <v>17</v>
-      </c>
-      <c r="E129" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B130" s="1">
-        <v>45671</v>
+        <v>45768</v>
       </c>
       <c r="C130" s="1">
-        <v>45689</v>
-      </c>
-      <c r="D130" t="s">
-        <v>19</v>
-      </c>
-      <c r="E130" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B131" s="1">
-        <v>45671</v>
+        <v>45768</v>
       </c>
       <c r="C131" s="1">
-        <v>45689</v>
-      </c>
-      <c r="D131" t="s">
-        <v>19</v>
-      </c>
-      <c r="E131" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B132" s="1">
         <v>45768</v>
       </c>
       <c r="C132" s="1">
-        <v>45806</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>45835</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>4</v>
+      </c>
+      <c r="B133" s="1">
+        <v>45862</v>
+      </c>
+      <c r="C133" s="1">
+        <v>45897</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>5</v>
       </c>
-      <c r="B133" s="1">
-        <v>45768</v>
-      </c>
-      <c r="C133" s="1">
-        <v>45806</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="B134" s="1">
+        <v>45862</v>
+      </c>
+      <c r="C134" s="1">
+        <v>45897</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>6</v>
       </c>
-      <c r="B134" s="1">
-        <v>45768</v>
-      </c>
-      <c r="C134" s="1">
-        <v>45806</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="B135" s="1">
+        <v>45862</v>
+      </c>
+      <c r="C135" s="1">
+        <v>45897</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>7</v>
       </c>
-      <c r="B135" s="1">
-        <v>45768</v>
-      </c>
-      <c r="C135" s="1">
-        <v>45806</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>8</v>
-      </c>
       <c r="B136" s="1">
-        <v>45768</v>
+        <v>45862</v>
       </c>
       <c r="C136" s="1">
-        <v>45835</v>
+        <v>45897</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B137" s="1">
         <v>45862</v>
       </c>
       <c r="C137" s="1">
-        <v>45897</v>
+        <v>45912</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B138" s="1">
-        <v>45862</v>
+        <v>45580</v>
       </c>
       <c r="C138" s="1">
-        <v>45897</v>
+        <v>45602</v>
+      </c>
+      <c r="D138" t="s">
+        <v>10</v>
+      </c>
+      <c r="E138" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B139" s="1">
-        <v>45862</v>
+        <v>45580</v>
       </c>
       <c r="C139" s="1">
-        <v>45897</v>
+        <v>45609</v>
+      </c>
+      <c r="D139" t="s">
+        <v>10</v>
+      </c>
+      <c r="E139" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B140" s="1">
-        <v>45862</v>
+        <v>45580</v>
       </c>
       <c r="C140" s="1">
-        <v>45897</v>
+        <v>45602</v>
+      </c>
+      <c r="D140" t="s">
+        <v>10</v>
+      </c>
+      <c r="E140" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B141" s="1">
-        <v>45862</v>
+        <v>45580</v>
       </c>
       <c r="C141" s="1">
-        <v>45912</v>
+        <v>45609</v>
+      </c>
+      <c r="D141" t="s">
+        <v>10</v>
+      </c>
+      <c r="E141" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>25</v>
+      </c>
+      <c r="B142" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C142" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D142" t="s">
+        <v>13</v>
+      </c>
+      <c r="E142" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>27</v>
+      </c>
+      <c r="B143" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C143" s="1">
+        <v>45609</v>
+      </c>
+      <c r="D143" t="s">
+        <v>13</v>
+      </c>
+      <c r="E143" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>25</v>
+      </c>
+      <c r="B144" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C144" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D144" t="s">
+        <v>13</v>
+      </c>
+      <c r="E144" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>27</v>
+      </c>
+      <c r="B145" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C145" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D145" t="s">
+        <v>13</v>
+      </c>
+      <c r="E145" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>25</v>
+      </c>
+      <c r="B146" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C146" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D146" t="s">
+        <v>14</v>
+      </c>
+      <c r="E146" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>27</v>
+      </c>
+      <c r="B147" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C147" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D147" t="s">
+        <v>14</v>
+      </c>
+      <c r="E147" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>25</v>
+      </c>
+      <c r="B148" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C148" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D148" t="s">
+        <v>14</v>
+      </c>
+      <c r="E148" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>27</v>
+      </c>
+      <c r="B149" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C149" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D149" t="s">
+        <v>14</v>
+      </c>
+      <c r="E149" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>25</v>
+      </c>
+      <c r="B150" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C150" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D150" t="s">
+        <v>18</v>
+      </c>
+      <c r="E150" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>27</v>
+      </c>
+      <c r="B151" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C151" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D151" t="s">
+        <v>18</v>
+      </c>
+      <c r="E151" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>25</v>
+      </c>
+      <c r="B152" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C152" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D152" t="s">
+        <v>18</v>
+      </c>
+      <c r="E152" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>27</v>
+      </c>
+      <c r="B153" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C153" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D153" t="s">
+        <v>18</v>
+      </c>
+      <c r="E153" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>25</v>
+      </c>
+      <c r="B154" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C154" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D154" t="s">
+        <v>20</v>
+      </c>
+      <c r="E154" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>27</v>
+      </c>
+      <c r="B155" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C155" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D155" t="s">
+        <v>20</v>
+      </c>
+      <c r="E155" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>25</v>
+      </c>
+      <c r="B156" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C156" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D156" t="s">
+        <v>20</v>
+      </c>
+      <c r="E156" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>27</v>
+      </c>
+      <c r="B157" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C157" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D157" t="s">
+        <v>20</v>
+      </c>
+      <c r="E157" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>25</v>
+      </c>
+      <c r="B158" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C158" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D158" t="s">
+        <v>16</v>
+      </c>
+      <c r="E158" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>27</v>
+      </c>
+      <c r="B159" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C159" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D159" t="s">
+        <v>16</v>
+      </c>
+      <c r="E159" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>25</v>
+      </c>
+      <c r="B160" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C160" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D160" t="s">
+        <v>15</v>
+      </c>
+      <c r="E160" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>27</v>
+      </c>
+      <c r="B161" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C161" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D161" t="s">
+        <v>15</v>
+      </c>
+      <c r="E161" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>25</v>
+      </c>
+      <c r="B162" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C162" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D162" t="s">
+        <v>17</v>
+      </c>
+      <c r="E162" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>27</v>
+      </c>
+      <c r="B163" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C163" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D163" t="s">
+        <v>17</v>
+      </c>
+      <c r="E163" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>25</v>
+      </c>
+      <c r="B164" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C164" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D164" t="s">
+        <v>19</v>
+      </c>
+      <c r="E164" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>27</v>
+      </c>
+      <c r="B165" s="1">
+        <v>45582</v>
+      </c>
+      <c r="C165" s="1">
+        <v>45603</v>
+      </c>
+      <c r="D165" t="s">
+        <v>19</v>
+      </c>
+      <c r="E165" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B136" xr:uid="{89A68A17-021F-4C89-9F43-C50D4EDC1708}">
-    <filterColumn colId="0">
-      <filters>
-        <dateGroupItem year="2025" month="7" dateTimeGrouping="month"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:B165" xr:uid="{89A68A17-021F-4C89-9F43-C50D4EDC1708}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>